<commit_message>
Change titles in table
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -548,37 +548,37 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>Jan-2020</t>
+          <t>Jan</t>
         </is>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>Feb-2020</t>
+          <t>Feb</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>Mar-2020</t>
+          <t>Mar</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>Apr-2020</t>
+          <t>Apr</t>
         </is>
       </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
-          <t>May-2020</t>
+          <t>May</t>
         </is>
       </c>
       <c r="K6" s="2" t="inlineStr">
         <is>
-          <t>Jun-2020</t>
+          <t>Jun</t>
         </is>
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>Reporting_Period_Total</t>
+          <t>YTD Total</t>
         </is>
       </c>
     </row>

</xml_diff>